<commit_message>
Added: Buscador de tickets
</commit_message>
<xml_diff>
--- a/[docs]/Categoria de tickets.xlsx
+++ b/[docs]/Categoria de tickets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\[proyectos]\HelpFlow\[docs]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5FFB360-B9CE-4FA3-8386-81E695272287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28FFA16-55F9-4228-B0E4-B74A8C8E7F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5A98425E-ACAC-4E26-87A3-7833B29989B1}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5A98425E-ACAC-4E26-87A3-7833B29989B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Problemas de hardware</t>
   </si>

</xml_diff>